<commit_message>
completely change the way teams are built
</commit_message>
<xml_diff>
--- a/src/main/resources/players.xlsx
+++ b/src/main/resources/players.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohrk/source/min-conflict-rand-team/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01ABD8D9-D3EE-084E-86FC-E6B4F296626A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34EA38D9-3F7D-5146-98A2-9E627C7ED615}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27780" yWindow="600" windowWidth="10000" windowHeight="13500" xr2:uid="{6AD1AC6B-AB35-D04F-963A-7CA185F29C3B}"/>
+    <workbookView xWindow="860" yWindow="2700" windowWidth="32020" windowHeight="16940" xr2:uid="{6AD1AC6B-AB35-D04F-963A-7CA185F29C3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>Men</t>
-  </si>
-  <si>
-    <t>Women</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Bert</t>
   </si>
@@ -103,13 +97,25 @@
   </si>
   <si>
     <t>Ava</t>
+  </si>
+  <si>
+    <t>Upper Men</t>
+  </si>
+  <si>
+    <t>Upper Women</t>
+  </si>
+  <si>
+    <t>Lower Men</t>
+  </si>
+  <si>
+    <t>Lower Women</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -125,8 +131,16 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
-      <color rgb="FF008000"/>
+      <color theme="1"/>
       <name val="Menlo"/>
       <family val="2"/>
     </font>
@@ -151,10 +165,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,115 +484,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8022365B-D61E-B444-81F1-F6086F283898}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="42" customWidth="1"/>
+    <col min="4" max="4" width="53.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B12">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="C12">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <f>SUM(A12:D12)</f>
         <v>25</v>
       </c>
     </row>

</xml_diff>